<commit_message>
FINAL; cleanup; changed readme; added plots
</commit_message>
<xml_diff>
--- a/metrics/disk_usage.xlsx
+++ b/metrics/disk_usage.xlsx
@@ -456,7 +456,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>39.740234375</v>
+        <v>3.039337158203125</v>
       </c>
     </row>
     <row r="3">
@@ -476,7 +476,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>38.01848589628935</v>
+        <v>40.49220751598477</v>
       </c>
     </row>
     <row r="5">
@@ -486,7 +486,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>47.73055886477232</v>
+        <v>152.7227372182533</v>
       </c>
     </row>
   </sheetData>

</xml_diff>